<commit_message>
ISSUE-CELLSCLOUD-13528: Add remove text exmaples.
</commit_message>
<xml_diff>
--- a/examples/BookText.xlsx
+++ b/examples/BookText.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud.family\cells.cloud-sdk-python\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud.family\cells.cloud-4.0\src\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EBF216-6E4D-4C22-ADBD-3B8EC3F16840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A282621-1C14-42D7-9093-5EA6EAAAF1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="10" r:id="rId1"/>
-    <sheet name="HumanResources" sheetId="15" r:id="rId2"/>
-    <sheet name="SDKs" sheetId="11" r:id="rId3"/>
-    <sheet name="RawFormatData" sheetId="12" r:id="rId4"/>
-    <sheet name="Blank" sheetId="14" r:id="rId5"/>
-    <sheet name="Format" sheetId="13" r:id="rId6"/>
+    <sheet name="Bikes" sheetId="16" r:id="rId2"/>
+    <sheet name="HumanResources" sheetId="15" r:id="rId3"/>
+    <sheet name="SDKs" sheetId="11" r:id="rId4"/>
+    <sheet name="RawFormatData" sheetId="12" r:id="rId5"/>
+    <sheet name="Blank" sheetId="14" r:id="rId6"/>
+    <sheet name="Format" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Name_2">#REF!</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="175">
   <si>
     <t xml:space="preserve">   Hi,     RoY   Wang.  hellow  word!         
 </t>
@@ -438,6 +439,157 @@
   </si>
   <si>
     <t xml:space="preserve">    Sales      Director      Assistant</t>
+  </si>
+  <si>
+    <t>Bike is bike.</t>
+  </si>
+  <si>
+    <t>From heritage steel commuters to UCI-level carbon racers, these 16 labels cover every rider and budget on the 2025 market.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Below are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>16 major bicycle brands</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> that dominate shops and podiums in 2025, each with a one-line snapshot of what they’re best known for.</t>
+    </r>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>One-line Intro</t>
+  </si>
+  <si>
+    <t>Taiwan’s world-beater; largest bike maker on Earth, famed for stiff-yet-light alloy &amp; carbon road and MTB rigs</t>
+  </si>
+  <si>
+    <t>Also out of Taiwan; sponsors WorldTour pro-teams and builds bullet-proof alloy frames for every discipline</t>
+  </si>
+  <si>
+    <t>American premium icon; birthplace of OCLV carbon, lifetime warranty, and the Madone aero road series</t>
+  </si>
+  <si>
+    <t>California tech-heavy brand that gave the world the Stumpjumper (first production MTB) and wind-tunnel-proven Tarmac.</t>
+  </si>
+  <si>
+    <t>Shenzhen powerhouse; 10-million-bike annual capacity, carbon-fibre expert and value-priced global OEM.</t>
+  </si>
+  <si>
+    <t>China’s 1897-born heritage name; classic city bikes and now e-bikes sold in 50+ countries.</t>
+  </si>
+  <si>
+    <t>Shanghai stalwart since 1940; once made the national “standard” bike and still cranks out commuters and e-cycles</t>
+  </si>
+  <si>
+    <t>Tianjin’s 1950 legacy marque; bright-coloured Dutch-style city bikes that roll off at 1 million+ units a year.</t>
+  </si>
+  <si>
+    <t>Tianjin Fuji-ta’s house brand; high-tensile steel work-horses rated to 150 kg and priced for the masses</t>
+  </si>
+  <si>
+    <t>French sports hyper-market; B’Twin and Rockrider lines give Euro-certified performance at supermarket prices</t>
+  </si>
+  <si>
+    <t>Guangzhou 1992-born factory; entry-level to mid-range MTB and gravel bikes exported to 60+ countries</t>
+  </si>
+  <si>
+    <t>Inventor of the modern folding bike (1982); 400+ patents, folds in 15 s, global commuter favourite</t>
+  </si>
+  <si>
+    <t>Taiwan 1966 originator; stylish folders with patented 3-step lock, loved by urban rail riders</t>
+  </si>
+  <si>
+    <t>SAVA</t>
+  </si>
+  <si>
+    <t>German-design team, Chinese carbon plant; ultralight road and gravel rigs under 1 kg frame weight</t>
+  </si>
+  <si>
+    <t>EROADE</t>
+  </si>
+  <si>
+    <t>German-engineered, China-built; belt-drive and carbon belt folders pitched as “fast as wind” commuters</t>
+  </si>
+  <si>
+    <t>Tern</t>
+  </si>
+  <si>
+    <t>Taiwan start-up (2011) focusing on micro-mobility; ultra-compact fold and e-folder lines for multi-modal cities</t>
+  </si>
+  <si>
+    <t>GIANT</t>
+  </si>
+  <si>
+    <t>MERIDA</t>
+  </si>
+  <si>
+    <t>TREK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialized </t>
+  </si>
+  <si>
+    <t>XDS</t>
+  </si>
+  <si>
+    <t>PHOENIX</t>
+  </si>
+  <si>
+    <t>Forever</t>
+  </si>
+  <si>
+    <t>FLYING PIGEON</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BATTLE</t>
+  </si>
+  <si>
+    <t>DECATHLON</t>
+  </si>
+  <si>
+    <t>TRINX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAHON </t>
+  </si>
+  <si>
+    <t>OYAMA</t>
+  </si>
+  <si>
+    <t>Hi, Aspose Cells Cloud Welcomes You!</t>
+  </si>
+  <si>
+    <t>Hi, aspose cells cloud welcomes you!</t>
+  </si>
+  <si>
+    <t>hi, aspose cells cloud welcomes you!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi, Aspose Cells Cloud welcomes you!
+</t>
+  </si>
+  <si>
+    <t>AAB;AAC;AAA;AAB;BBA;BAC;AAC</t>
+  </si>
+  <si>
+    <t>AAB;AAC;AAA;AaB;BBA;BAC;aac</t>
   </si>
 </sst>
 </file>
@@ -450,7 +602,7 @@
     <numFmt numFmtId="166" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +637,27 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -506,7 +679,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -625,8 +798,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -634,8 +866,9 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -701,14 +934,59 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -716,6 +994,7 @@
     <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1240,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2036091A-1B06-4FA8-8B01-7CDD0E466B74}">
-  <dimension ref="D4:P12"/>
+  <dimension ref="D4:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1257,56 +1536,373 @@
       </c>
     </row>
     <row r="6" spans="4:16">
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
     </row>
     <row r="7" spans="4:16">
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
     </row>
     <row r="10" spans="4:16">
       <c r="D10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:16">
+    <row r="11" spans="4:16" ht="15" customHeight="1">
       <c r="D11">
         <v>2</v>
       </c>
+      <c r="J11" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
     </row>
     <row r="12" spans="4:16">
       <c r="D12">
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="4:16">
+      <c r="J13" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+    </row>
+    <row r="14" spans="4:16">
+      <c r="J14" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+    </row>
+    <row r="15" spans="4:16">
+      <c r="J15" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+    </row>
+    <row r="16" spans="4:16">
+      <c r="J16" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="J16:P16"/>
     <mergeCell ref="J6:P6"/>
     <mergeCell ref="J7:P7"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="J13:P13"/>
+    <mergeCell ref="J14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D3A14B-C57D-4640-BC1F-6DDB015F19CC}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="78.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" thickBot="1">
+      <c r="A2" s="23"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A3" s="24"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="26"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A6" s="27"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+      <c r="B7" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B8" s="34">
+        <v>1</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B9" s="34">
+        <v>2</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B10" s="34">
+        <v>3</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B11" s="30">
+        <v>4</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30.75" thickBot="1">
+      <c r="B12" s="30">
+        <v>5</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B13" s="30">
+        <v>6</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B14" s="34">
+        <v>7</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30.75" thickBot="1">
+      <c r="B15" s="30">
+        <v>8</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B16" s="34">
+        <v>9</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B17" s="34">
+        <v>10</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B18" s="34">
+        <v>11</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B19" s="34">
+        <v>12</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B20" s="34">
+        <v>13</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B21" s="34">
+        <v>14</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="29.25" thickBot="1">
+      <c r="B22" s="34">
+        <v>15</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.5">
+      <c r="B23" s="34">
+        <v>16</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="165">
+      <c r="A24" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:D4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D12" r:id="rId1" display="http://www.360doc.com/content/24/0618/14/68688584_1126524051.shtml" xr:uid="{8D947FD2-02B5-43F7-BBC3-7889E7CBAB6E}"/>
+    <hyperlink ref="D15" r:id="rId2" display="https://m.chinabgao.com/top/brand/78492.html" xr:uid="{11329605-FA50-42A2-B2AA-6B7E88696855}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36E46D4-F869-43BB-BCF6-AF7C486C806E}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1441,7 +2037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7700EC40-302C-4CF3-84D8-CC1D43AB38CF}">
   <dimension ref="B2:B9"/>
   <sheetViews>
@@ -1510,7 +2106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2C4DD6-AAA4-4047-B9C0-2794487807E2}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -2197,7 +2793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C88BA-98B2-4FD4-8ACD-5DC03F8E0944}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2209,7 +2805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCB97A3-2C26-4389-8789-5602194E36D3}">
   <dimension ref="A2:D44"/>
   <sheetViews>

</xml_diff>